<commit_message>
Oggi sto push push
</commit_message>
<xml_diff>
--- a/AnalisiCWE.xlsx
+++ b/AnalisiCWE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefano/Desktop/SecureCodeAI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA3EFD89-8933-374D-BC3C-C123470D85CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7461A7F7-B2A8-2A4E-9B07-EFF0437BC7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="2900" windowWidth="30360" windowHeight="17440" activeTab="2" xr2:uid="{5A294F49-F358-D048-AA4E-3EF54D28B781}"/>
+    <workbookView xWindow="1880" yWindow="1660" windowWidth="32580" windowHeight="18940" activeTab="3" xr2:uid="{5A294F49-F358-D048-AA4E-3EF54D28B781}"/>
   </bookViews>
   <sheets>
     <sheet name="Bandit_ChatGPT" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CodeQL_ChatGPT" sheetId="3" r:id="rId3"/>
     <sheet name="CodeQL_Copilot" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="75">
   <si>
     <t>CWE</t>
   </si>
@@ -53,12 +53,12 @@
     <t>note_SENZA</t>
   </si>
   <si>
+    <t>tar.extractall used without validation</t>
+  </si>
+  <si>
     <t>Note_CON</t>
   </si>
   <si>
-    <t>tar.extractall used without validation</t>
-  </si>
-  <si>
     <t>5 start proc with shell + 2 subprocess popen with shell=True</t>
   </si>
   <si>
@@ -110,21 +110,9 @@
     <t>Tipo</t>
   </si>
   <si>
-    <t>Path Injection</t>
-  </si>
-  <si>
     <t>+2 CWE-200 (stack_trace_exposure)</t>
   </si>
   <si>
-    <t>+4 CWE-259 (Hardcoded Credentials)</t>
-  </si>
-  <si>
-    <t>+2 Cwe-259 (Hardcoded Credentials)</t>
-  </si>
-  <si>
-    <t>ma non viene effettuato controllo valido sulle estensioni dei file +6 CWE-22 + 4 URL Redirection + 2 CWE-74 (Reflective XSS) + 1 CWE-259 (Hardcoded Credentials)</t>
-  </si>
-  <si>
     <t>+5 CWE-200 (stack_trace_exposure) + 2 CWE-74 (reflective XSS / Code injection)</t>
   </si>
   <si>
@@ -146,16 +134,136 @@
     <t>+1 CWE-601 (URL Redirection)</t>
   </si>
   <si>
-    <t>+15 CWE-601 (URL Redirection) + 2 Path Injection ma sanificate + Hardcoded Credential (controlla codice)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 CWE-200 (Stack Trace Exposure) </t>
-  </si>
-  <si>
-    <t>Unsafe Deseralization</t>
+    <t xml:space="preserve">1 ma input validato + 6 CWE-200 (Stack Trace Exposure) </t>
   </si>
   <si>
     <t>+1 CWE-200 (stack trace exposure)</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Improper Input Validation</t>
+  </si>
+  <si>
+    <t>4 CWE-601 (URL Redirection) + 3 CWE-664 (Flask Debug)</t>
+  </si>
+  <si>
+    <t>Path Traversal</t>
+  </si>
+  <si>
+    <t>2 CWE-664 (Flask Debug)</t>
+  </si>
+  <si>
+    <t>OS Command Injection</t>
+  </si>
+  <si>
+    <t>3 CWE-664 (Flask Debug)</t>
+  </si>
+  <si>
+    <t>Cross-site Scripting</t>
+  </si>
+  <si>
+    <t>4 CWE-664 (Flask Debug)</t>
+  </si>
+  <si>
+    <t>SQL Injection</t>
+  </si>
+  <si>
+    <t>7 CWE-664 (Flask Debug)</t>
+  </si>
+  <si>
+    <t>Buffer Overflow</t>
+  </si>
+  <si>
+    <t>Out-of-bounds Read</t>
+  </si>
+  <si>
+    <t>Integer Overflow or Wraparound</t>
+  </si>
+  <si>
+    <t>Information Disclosure</t>
+  </si>
+  <si>
+    <t>Missing Authentication for Critical Function</t>
+  </si>
+  <si>
+    <t>Use After Free</t>
+  </si>
+  <si>
+    <t>Unrestricted File Upload</t>
+  </si>
+  <si>
+    <t>NULL Pointer Dereference</t>
+  </si>
+  <si>
+    <t>Deserialization of Untrusted Data</t>
+  </si>
+  <si>
+    <t>Insufficiently Protected Credentials</t>
+  </si>
+  <si>
+    <t>Incorrect Permission Assignment for Critical Resource</t>
+  </si>
+  <si>
+    <t>Out-of-bounds Write</t>
+  </si>
+  <si>
+    <t>4 (password messa in chiaro nel codice)</t>
+  </si>
+  <si>
+    <t>Use of Hard-coded Credentials</t>
+  </si>
+  <si>
+    <t>+ 7 CWE-664(Flask Debug) + 2 CWE-200 (stack trace exposure) + CWE-74(code injection) + CWE-798 (Hardcoded credential)</t>
+  </si>
+  <si>
+    <t>ma non viene effettuato controllo su estensione file + 5 CWE-664 (Flask Debug) + 4 CWE-22 (path Injection) + 4 CWE-601 (url-redirection) + 1 CWE-798 (hardcoded credential)</t>
+  </si>
+  <si>
+    <t>5 CWE-665 (Flask Debug) + 2 CWE-798 (hardcoded credential) + CWE-79 (reflective-xss)</t>
+  </si>
+  <si>
+    <t>2 CWE-798 (hardcoded credential) + 7 CWE-664 (Flask Debug)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ 4 CWE-664 (Flask Debug) </t>
+  </si>
+  <si>
+    <t>+4 CWE-798 (Hardcoded Credentials)</t>
+  </si>
+  <si>
+    <t>+2 Cwe-798 (Hardcoded Credentials)</t>
+  </si>
+  <si>
+    <t>ma non viene effettuato controllo valido sulle estensioni dei file +6 CWE-22 + 4 URL Redirection + 2 CWE-74 (Reflective XSS) + 1 CWE-798 (Hardcoded Credentials)</t>
+  </si>
+  <si>
+    <t>+15 CWE-601 (URL Redirection) + 2 Path Injection ma sanificate + CWE-798 Hardcoded Credential (controlla codice)</t>
+  </si>
+  <si>
+    <t>+CWE-200(Stack trace exposure)</t>
+  </si>
+  <si>
+    <t>3 CWE-601 (URL redirection) + CWE-200 (stack trace exposure)</t>
+  </si>
+  <si>
+    <t>1 "path-injection" ma input sanificato + 2 "tarslip" ma file validati dopo estrazione</t>
+  </si>
+  <si>
+    <t>+3 CWE-200 (stack-trace-exposure)</t>
+  </si>
+  <si>
+    <t>+1 CWE-200 (stack-trace-exposure)</t>
+  </si>
+  <si>
+    <t>+ CWE-798 (hardcoded credential)</t>
+  </si>
+  <si>
+    <t>+ 7 CWE-601 (url redirection) + 2 CWE-200 (stack-trace-exposure) + 1 CWE-798 (hardcoded credential - ma è exaple usage)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 ma consiglia di validare l'input prima + 6 CWE-200 (Stack Trace Exposure) </t>
   </si>
 </sst>
 </file>
@@ -199,24 +307,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -556,23 +665,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{420EADCB-EDB9-C34A-B4FB-FDE09DC18981}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="11.1640625" style="1"/>
+    <col min="2" max="2" width="37.1640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="4" width="48.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="37.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="1"/>
     <col min="6" max="6" width="14" style="1" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="33" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,13 +696,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>20</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
@@ -600,15 +713,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>22</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -617,10 +733,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>78</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="C4" s="1">
         <v>7</v>
       </c>
@@ -634,10 +753,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>79</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
@@ -648,10 +770,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>89</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="C6" s="1">
         <v>0</v>
       </c>
@@ -659,10 +784,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>119</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="C7" s="1">
         <v>0</v>
       </c>
@@ -670,10 +798,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>125</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="C8" s="1">
         <v>0</v>
       </c>
@@ -681,10 +812,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>190</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="C9" s="1">
         <v>0</v>
       </c>
@@ -692,10 +826,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>200</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="C10" s="1">
         <v>0</v>
       </c>
@@ -703,10 +840,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>306</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="C11" s="1">
         <v>0</v>
       </c>
@@ -714,10 +854,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>416</v>
       </c>
+      <c r="B12" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="C12" s="1">
         <v>0</v>
       </c>
@@ -727,12 +870,14 @@
       <c r="F12" s="1">
         <v>0</v>
       </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>434</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="C13" s="1">
         <v>0</v>
       </c>
@@ -740,10 +885,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>476</v>
       </c>
+      <c r="B14" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C14" s="1">
         <v>0</v>
       </c>
@@ -751,10 +899,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>502</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
@@ -762,10 +913,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>522</v>
       </c>
+      <c r="B16" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
@@ -779,10 +933,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>732</v>
       </c>
+      <c r="B17" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="C17" s="1">
         <v>0</v>
       </c>
@@ -790,10 +947,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>787</v>
       </c>
+      <c r="B18" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C18" s="1">
         <v>0</v>
       </c>
@@ -801,12 +961,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>798</v>
       </c>
+      <c r="B19" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="C19" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -822,19 +985,20 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="29.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="79.83203125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="51.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="59.33203125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="37.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,13 +1012,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>20</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
@@ -862,10 +1029,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>22</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C3" s="1">
         <v>3</v>
       </c>
@@ -879,10 +1049,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>78</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="C4" s="1">
         <v>6</v>
       </c>
@@ -896,10 +1069,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>79</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -910,10 +1086,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>89</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="C6" s="1">
         <v>0</v>
       </c>
@@ -924,10 +1103,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>119</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="C7" s="1">
         <v>0</v>
       </c>
@@ -935,10 +1117,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>125</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="C8" s="1">
         <v>0</v>
       </c>
@@ -946,10 +1131,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>190</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="C9" s="1">
         <v>0</v>
       </c>
@@ -957,10 +1145,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>200</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="C10" s="1">
         <v>0</v>
       </c>
@@ -971,10 +1162,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>306</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="C11" s="1">
         <v>0</v>
       </c>
@@ -985,10 +1179,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>416</v>
       </c>
+      <c r="B12" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="C12" s="1">
         <v>0</v>
       </c>
@@ -1002,10 +1199,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>434</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="C13" s="1">
         <v>0</v>
       </c>
@@ -1016,10 +1216,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>476</v>
       </c>
+      <c r="B14" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C14" s="1">
         <v>0</v>
       </c>
@@ -1027,10 +1230,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>502</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
@@ -1041,22 +1247,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>522</v>
       </c>
+      <c r="B16" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="D16" s="4"/>
       <c r="F16" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>732</v>
       </c>
+      <c r="B17" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="C17" s="1">
         <v>0</v>
       </c>
@@ -1064,10 +1276,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>787</v>
       </c>
+      <c r="B18" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C18" s="1">
         <v>0</v>
       </c>
@@ -1075,18 +1290,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>798</v>
       </c>
+      <c r="B19" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="C19" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>7</v>
@@ -1101,20 +1319,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7B8CBE-637F-4340-803F-36E0323F3B1D}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="19.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="29.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="43.5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="43.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="1"/>
     <col min="6" max="6" width="15.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.1640625" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="33.1640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1127,102 +1345,117 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>4</v>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>20</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1">
         <v>4</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>30</v>
+      <c r="G3" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>78</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>24</v>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>31</v>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>79</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>3</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>89</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C6" s="1">
         <v>0</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>119</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C7" s="1">
         <v>0</v>
       </c>
@@ -1230,10 +1463,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>125</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C8" s="1">
         <v>0</v>
       </c>
@@ -1241,9 +1477,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>190</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -1256,39 +1495,48 @@
       <c r="A10" s="1">
         <v>200</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="C10" s="1">
         <v>0</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>25</v>
+      <c r="D10" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="G10" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>306</v>
       </c>
+      <c r="B11" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C11" s="1">
         <v>0</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>26</v>
+      <c r="D11" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>416</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
@@ -1301,22 +1549,28 @@
       <c r="A13" s="1">
         <v>434</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="C13" s="1">
         <v>0</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>27</v>
+      <c r="D13" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>476</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -1330,39 +1584,45 @@
         <v>502</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>28</v>
+      <c r="D15" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="G15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>522</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>732</v>
       </c>
+      <c r="B17" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="C17" s="1">
         <v>0</v>
       </c>
@@ -1370,9 +1630,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>787</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -1385,11 +1648,14 @@
       <c r="A19" s="1">
         <v>798</v>
       </c>
+      <c r="B19" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1401,124 +1667,339 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED45727F-56D0-B348-AB08-17D05F7A2D8D}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="27" style="3" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="30.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="37.83203125" style="5" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="26.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>119</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>190</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>306</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>416</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>434</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>476</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>502</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>522</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>732</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>787</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>798</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gemma excel file updated
</commit_message>
<xml_diff>
--- a/AnalisiCWE.xlsx
+++ b/AnalisiCWE.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefano/Desktop/SecureCodeAI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tonyb\OneDrive\Desktop\SecureCodeAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA4D156-6192-394F-BC68-843816B064BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93837051-A383-4CFC-B9AD-2DCB5CF8D800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="20960" activeTab="2" xr2:uid="{5A294F49-F358-D048-AA4E-3EF54D28B781}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5A294F49-F358-D048-AA4E-3EF54D28B781}"/>
   </bookViews>
   <sheets>
     <sheet name="Bandit_ChatGPT" sheetId="1" r:id="rId1"/>
     <sheet name="Bandit_Copilot" sheetId="2" r:id="rId2"/>
     <sheet name="CodeQL_ChatGPT" sheetId="3" r:id="rId3"/>
     <sheet name="CodeQL_Copilot" sheetId="4" r:id="rId4"/>
+    <sheet name="Foglio1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="76">
   <si>
     <t>CWE</t>
   </si>
@@ -234,13 +235,46 @@
   </si>
   <si>
     <t>password put in clear text in the code</t>
+  </si>
+  <si>
+    <t>COPILOT</t>
+  </si>
+  <si>
+    <t>BANDIT</t>
+  </si>
+  <si>
+    <t>CODEQL</t>
+  </si>
+  <si>
+    <t>NO BP</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>GPT+BP</t>
+  </si>
+  <si>
+    <t>COPILOT+BP</t>
+  </si>
+  <si>
+    <t>CHATGPT</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -256,8 +290,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,6 +322,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -295,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -327,6 +373,8 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -663,24 +711,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{420EADCB-EDB9-C34A-B4FB-FDE09DC18981}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E37" sqref="E37"/>
+      <selection pane="topRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.69921875" style="3" customWidth="1"/>
     <col min="2" max="2" width="29.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.19921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" style="3" customWidth="1"/>
     <col min="5" max="5" width="33" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.69921875" style="3" customWidth="1"/>
     <col min="7" max="7" width="33" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.1640625" style="4"/>
+    <col min="8" max="16384" width="11.19921875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -703,7 +751,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>20</v>
       </c>
@@ -720,7 +768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>22</v>
       </c>
@@ -743,7 +791,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>78</v>
       </c>
@@ -766,7 +814,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>79</v>
       </c>
@@ -786,7 +834,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>89</v>
       </c>
@@ -803,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>119</v>
       </c>
@@ -820,7 +868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>125</v>
       </c>
@@ -837,7 +885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>190</v>
       </c>
@@ -854,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>200</v>
       </c>
@@ -871,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>306</v>
       </c>
@@ -888,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>416</v>
       </c>
@@ -908,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>434</v>
       </c>
@@ -925,7 +973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>476</v>
       </c>
@@ -942,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>502</v>
       </c>
@@ -959,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>522</v>
       </c>
@@ -982,7 +1030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>732</v>
       </c>
@@ -999,7 +1047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>787</v>
       </c>
@@ -1016,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>798</v>
       </c>
@@ -1042,24 +1090,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3810DE5B-4527-1E4E-AE98-902099D06CA0}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C33" sqref="C33"/>
+      <selection pane="topRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3"/>
-    <col min="2" max="2" width="29.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="3"/>
+    <col min="2" max="2" width="29.296875" style="2" customWidth="1"/>
     <col min="3" max="3" width="13" style="2" customWidth="1"/>
     <col min="4" max="4" width="13" style="3" customWidth="1"/>
     <col min="5" max="5" width="33" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.796875" style="3" customWidth="1"/>
     <col min="7" max="7" width="33" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="4"/>
+    <col min="8" max="16384" width="8.796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1130,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>20</v>
       </c>
@@ -1099,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="61.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>22</v>
       </c>
@@ -1119,7 +1167,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="88" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="88.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>78</v>
       </c>
@@ -1142,7 +1190,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>79</v>
       </c>
@@ -1162,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>89</v>
       </c>
@@ -1179,7 +1227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>119</v>
       </c>
@@ -1196,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>125</v>
       </c>
@@ -1213,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>190</v>
       </c>
@@ -1230,7 +1278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>200</v>
       </c>
@@ -1247,7 +1295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>306</v>
       </c>
@@ -1264,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>416</v>
       </c>
@@ -1287,7 +1335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>434</v>
       </c>
@@ -1304,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>476</v>
       </c>
@@ -1321,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>502</v>
       </c>
@@ -1338,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>522</v>
       </c>
@@ -1356,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>732</v>
       </c>
@@ -1373,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>787</v>
       </c>
@@ -1390,7 +1438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>798</v>
       </c>
@@ -1419,24 +1467,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7B8CBE-637F-4340-803F-36E0323F3B1D}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B23" sqref="B23"/>
+      <selection pane="topRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3"/>
-    <col min="2" max="2" width="29.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="3"/>
+    <col min="2" max="2" width="29.296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.19921875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.796875" style="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="3" customWidth="1"/>
     <col min="7" max="7" width="33" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="3"/>
+    <col min="8" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +1507,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>20</v>
       </c>
@@ -1482,7 +1530,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>22</v>
       </c>
@@ -1505,7 +1553,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>78</v>
       </c>
@@ -1528,7 +1576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>79</v>
       </c>
@@ -1548,7 +1596,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>89</v>
       </c>
@@ -1568,7 +1616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>119</v>
       </c>
@@ -1585,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>125</v>
       </c>
@@ -1602,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>190</v>
       </c>
@@ -1619,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>200</v>
       </c>
@@ -1642,7 +1690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>306</v>
       </c>
@@ -1665,7 +1713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>416</v>
       </c>
@@ -1682,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>434</v>
       </c>
@@ -1705,7 +1753,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>476</v>
       </c>
@@ -1722,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>502</v>
       </c>
@@ -1745,7 +1793,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>522</v>
       </c>
@@ -1765,7 +1813,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>732</v>
       </c>
@@ -1782,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>787</v>
       </c>
@@ -1799,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>798</v>
       </c>
@@ -1827,21 +1875,21 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D26" sqref="D26"/>
+      <selection pane="topRight" activeCell="D19" activeCellId="3" sqref="E4 D3 D5 D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3"/>
-    <col min="2" max="2" width="29.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="3"/>
+    <col min="2" max="2" width="29.296875" style="2" customWidth="1"/>
     <col min="3" max="4" width="13" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="3" customWidth="1"/>
-    <col min="7" max="7" width="33.1640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="3"/>
+    <col min="7" max="7" width="33.19921875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1864,7 +1912,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>20</v>
       </c>
@@ -1887,7 +1935,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>22</v>
       </c>
@@ -1910,7 +1958,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>78</v>
       </c>
@@ -1930,7 +1978,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>79</v>
       </c>
@@ -1953,7 +2001,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>89</v>
       </c>
@@ -1973,7 +2021,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>119</v>
       </c>
@@ -1990,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>125</v>
       </c>
@@ -2007,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>190</v>
       </c>
@@ -2024,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>200</v>
       </c>
@@ -2044,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>306</v>
       </c>
@@ -2064,7 +2112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>416</v>
       </c>
@@ -2081,7 +2129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="85.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>434</v>
       </c>
@@ -2104,7 +2152,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>476</v>
       </c>
@@ -2118,7 +2166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>502</v>
       </c>
@@ -2141,7 +2189,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>522</v>
       </c>
@@ -2155,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>732</v>
       </c>
@@ -2172,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>787</v>
       </c>
@@ -2189,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>798</v>
       </c>
@@ -2210,6 +2258,75 @@
       </c>
       <c r="G19" s="1" t="s">
         <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11087EF7-C6FD-4670-9567-766425072EE8}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="11.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>